<commit_message>
added parser for SBI statements
</commit_message>
<xml_diff>
--- a/OLAP tables.xlsx
+++ b/OLAP tables.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiab\Projects\Expense Manager\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938C1362-86DD-44AF-8BD7-C2BB476B067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Budget_and_Expenses" sheetId="2" r:id="rId1"/>
+    <sheet name="Source_waste" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,10 +25,143 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>sub_category</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>budget_amount</t>
+  </si>
+  <si>
+    <t>expense_amount</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>C0013</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>C0014</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Vehicle payment</t>
+  </si>
+  <si>
+    <t>C0015</t>
+  </si>
+  <si>
+    <t>Maintainance</t>
+  </si>
+  <si>
+    <t>C0016</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>C0017</t>
+  </si>
+  <si>
+    <t>Repairs</t>
+  </si>
+  <si>
+    <t>C0018</t>
+  </si>
+  <si>
+    <t>Registration &amp; DMV</t>
+  </si>
+  <si>
+    <t>C0019</t>
+  </si>
+  <si>
+    <t>Public Transport</t>
+  </si>
+  <si>
+    <t>C0020</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Footwear</t>
+  </si>
+  <si>
+    <t>waste_amount</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>sub_source</t>
+  </si>
+  <si>
+    <t>XXXX-XXXX-4371</t>
+  </si>
+  <si>
+    <t>SBI</t>
+  </si>
+  <si>
+    <t>debit card</t>
+  </si>
+  <si>
+    <t>XXXX-XXXX-9967</t>
+  </si>
+  <si>
+    <t>SBI card</t>
+  </si>
+  <si>
+    <t>credit card</t>
+  </si>
+  <si>
+    <t>XXXXXXX2654</t>
+  </si>
+  <si>
+    <t>bank account</t>
+  </si>
+  <si>
+    <t>Internet Banking</t>
+  </si>
+  <si>
+    <t>expense_month</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +189,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +474,413 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C059351E-6029-490B-A135-F6A8F94DFF52}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44927</v>
+      </c>
+      <c r="F2" s="4">
+        <v>600</v>
+      </c>
+      <c r="G2" s="4">
+        <v>600</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44928</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2000</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2350</v>
+      </c>
+      <c r="H3" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44929</v>
+      </c>
+      <c r="F4" s="4">
+        <v>454</v>
+      </c>
+      <c r="G4" s="4">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44930</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2000</v>
+      </c>
+      <c r="H5" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44931</v>
+      </c>
+      <c r="F6" s="4">
+        <v>52</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44932</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5621</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44933</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44934</v>
+      </c>
+      <c r="F9" s="4">
+        <v>300</v>
+      </c>
+      <c r="G9" s="4">
+        <v>100</v>
+      </c>
+      <c r="H9" s="4">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E84CB77-0C5C-463B-A6C0-8AF5CC3FCC4D}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44927</v>
+      </c>
+      <c r="F2" s="4">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44928</v>
+      </c>
+      <c r="F3" s="4">
+        <v>8600</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44929</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45000</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44930</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3241</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E9" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>